<commit_message>
Updated upload.html - created an alert message in case the wrong file type is uploaded - in the preview area, created a table that has the headers of the excel file, the first row of data and the last row of data
</commit_message>
<xml_diff>
--- a/django-base/sampleExcel/xlsx_files/SampleDataExcel.xlsx
+++ b/django-base/sampleExcel/xlsx_files/SampleDataExcel.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sveta\source\repos\SMarhefka\IS601\django-base\sampleExcel\xlsx_files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2DEC6048-07AC-4058-B3A1-A96248045D32}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB47DAE4-72D6-4C1D-81EC-DAAE4648488B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1500" yWindow="1500" windowWidth="17280" windowHeight="8964" xr2:uid="{0CEE0D2C-EBA8-484A-BFFA-9525299E0D72}"/>
+    <workbookView xWindow="1152" yWindow="1152" windowWidth="11460" windowHeight="11184" xr2:uid="{0CEE0D2C-EBA8-484A-BFFA-9525299E0D72}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="14">
   <si>
     <t>first name</t>
   </si>
@@ -72,13 +72,19 @@
   </si>
   <si>
     <t>edmarhefka@comcast.net</t>
+  </si>
+  <si>
+    <t>date</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd;@"/>
+  </numFmts>
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -94,6 +100,12 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -103,7 +115,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -111,14 +123,33 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -434,15 +465,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F7E04D5F-B6CF-4BCE-AAEC-8222152B64BF}">
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="5" max="5" width="9.5546875" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -455,8 +489,11 @@
       <c r="D1" t="s">
         <v>3</v>
       </c>
+      <c r="E1" t="s">
+        <v>13</v>
+      </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -469,8 +506,11 @@
       <c r="D2">
         <v>13</v>
       </c>
+      <c r="E2" s="2">
+        <v>43882</v>
+      </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>7</v>
       </c>
@@ -483,8 +523,11 @@
       <c r="D3">
         <v>16</v>
       </c>
+      <c r="E3" s="2">
+        <v>43882</v>
+      </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>9</v>
       </c>
@@ -497,8 +540,11 @@
       <c r="D4">
         <v>33</v>
       </c>
+      <c r="E4" s="2">
+        <v>43886</v>
+      </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>11</v>
       </c>
@@ -510,6 +556,9 @@
       </c>
       <c r="D5">
         <v>50</v>
+      </c>
+      <c r="E5" s="3">
+        <v>43941</v>
       </c>
     </row>
   </sheetData>

</xml_diff>